<commit_message>
Automatische test-sync: 2025-06-22 17:08:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,8 +679,40 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Probleem met inloggen</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ik kan niet inloggen op mijn account. Kunnen jullie dit oplossen?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-06-22 17:08:10</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -700,7 +732,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -718,7 +750,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -748,6 +780,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 17:33:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -711,8 +711,281 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Geachte heer/mevrouw,
+Hartelijk dank voor uw sollicitatie voor de functie van marketeer. Ik zal uw CV zorgvuldig bekijken en zal spoedig contact met u opnemen.
+Met vriendelijke groet,
+[Naam]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-06-22 17:33:14</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Uitnodiging voor netwerkevent</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Graag nodig ik u uit voor ons zakelijke netwerkevent volgende maand.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Uitnodiging / Evenement</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Geachte heer/mevrouw,
+Hartelijk dank voor de uitnodiging voor het zakelijke netwerkevent volgende maand. Ik waardeer uw uitnodiging en zal graag aanwezig zijn.
+Met vriendelijke groet,
+[Uw naam]</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-06-22 17:33:17</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Probleem met inloggen</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Ik kan niet inloggen op mijn account. Kunnen jullie dit oplossen?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Hartelijk dank voor uw bericht. Om u beter van dienst te kunnen zijn, kunnen we u vragen om enkele gegevens te verstrekken, zoals uw accountnaam en eventuele foutmeldingen die u krijgt. Met deze informatie kunnen we het probleem identificeren en hopelijk snel voor u oplossen. U kunt dit sturen naar support@email.com. 
+Met vriendelijke groet,
+[Naam] 
+Klantenservice medewerker</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-06-22 17:33:19</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Beste,
+Bedankt voor je bericht. Onze openingstijden zijn van maandag tot en met vrijdag van 9.00 uur tot 18.00 uur. Op zaterdag zijn wij geopend van 10.00 uur tot 15.00 uur. Op zondag zijn wij gesloten.
+Met vriendelijke groet, 
+[Naam Bedrijf]</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-06-22 17:33:22</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Probleem met inloggen</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Ik kan niet inloggen op mijn account. Kunnen jullie dit oplossen?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Om je te kunnen helpen met het inlogprobleem op je account, hebben we wat meer informatie nodig. Kun je ons het e-mailadres en eventuele foutmeldingen die je krijgt sturen? We zullen ons best doen om zo snel mogelijk een oplossing te vinden.
+Met vriendelijke groet,
+[E-mailassistent]</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-06-22 17:33:24</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-06-22 17:33:25</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Beste [Naam],
+Dank voor je interesse in samenwerken aan een nieuw project. Graag ontvang ik meer details betreffende het project, zoals doelstellingen, tijdslijnen en verwachtingen. Op basis daarvan kunnen we een afspraak inplannen om de mogelijkheden te bespreken.
+Met vriendelijke groet,
+[Naam]</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-06-22 17:33:27</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -732,7 +1005,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -750,7 +1023,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -773,20 +1046,70 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Uitnodiging / Evenement</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 17:34:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$8</f>
+              <f>'Dashboard'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$8</f>
+              <f>'Dashboard'!$B$2:$B$9</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -984,8 +984,48 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Geachte heer/mevrouw,
+Hartelijk dank voor uw e-mail. Ik heb u bij deze afgemeld voor de nieuwsbrief. Mocht u in de toekomst weer interesse hebben, dan kunt u zich altijd opnieuw aanmelden.
+Met vriendelijke groet,
+[Naam]</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-06-22 17:34:14</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1005,7 +1045,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1023,7 +1063,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1113,6 +1153,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:42:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1024,8 +1024,40 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Stageverzoek</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Ik zoek een stageplek vanaf september. Is dit mogelijk bij jullie?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:42:15</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1045,7 +1077,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1096,17 +1128,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:43:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$9</f>
+              <f>'Dashboard'!$A$2:$A$10</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$9</f>
+              <f>'Dashboard'!$B$2:$B$10</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1056,8 +1056,49 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Beschadigd product ontvangen</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Het product dat ik heb ontvangen is beschadigd aangekomen.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Wat vervelend om te horen dat het product beschadigd is aangekomen. Kunt u ons meer details geven over de schade? Bijvoorbeeld, wat voor product is het en wat voor schade is er precies aan? Eventuele foto's van de schade kunnen ook nuttig zijn.
+Zodra we deze informatie hebben, zullen we ons best doen om een passende oplossing voor u te vinden.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:43:12</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1077,7 +1118,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1095,7 +1136,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1195,6 +1236,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:44:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$10</f>
+              <f>'Dashboard'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$10</f>
+              <f>'Dashboard'!$B$2:$B$11</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1097,8 +1097,49 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Wat is het verschil tussen product A en product B?</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw interesse in onze producten A en B. Het belangrijkste verschil tussen product A en B is de functionaliteit. Product A is ontworpen met functies zoals X, Y en Z, terwijl product B functies heeft zoals P, Q en R. Afhankelijk van uw behoeften en vereisten kunt u het product kiezen dat het beste bij uw situatie past.
+Als u meer gedetailleerde informatie nodig heeft over specifieke functies of kenmerken van product A en B, dan helpen wij u graag verder.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:44:13</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1118,7 +1159,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1136,7 +1177,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1246,6 +1287,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:45:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1138,8 +1138,40 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>MVO-beleid</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Hebben jullie een duurzaamheidsbeleid of MVO-doelen?</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:45:14</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1159,7 +1191,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1220,17 +1252,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Uitnodiging / Evenement</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1250,7 +1282,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Uitnodiging / Evenement</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1260,7 +1292,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1270,7 +1302,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1280,7 +1312,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1290,7 +1322,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B11" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:46:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1170,8 +1170,48 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Vragen over handleiding</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Waar kan ik de handleiding van product X vinden?</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw vraag. De handleiding van product X is te vinden op onze website onder de sectie 'Support' of 'Downloads'. Mocht u hier toch problemen mee ervaren, laat het ons dan weten zodat we u verder kunnen helpen.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:46:33</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1191,7 +1231,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1242,17 +1282,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:48:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$11</f>
+              <f>'Dashboard'!$A$2:$A$12</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$11</f>
+              <f>'Dashboard'!$B$2:$B$12</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1210,8 +1210,72 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>MVO-beleid</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Hebben jullie een duurzaamheidsbeleid of MVO-doelen?</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:47:57</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Bereikbaarheid klantenservice</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Hoe kan ik jullie het beste bereiken?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:48:30</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1231,7 +1295,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1249,7 +1313,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1302,17 +1366,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1332,7 +1396,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1352,7 +1416,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1366,6 +1430,16 @@
         </is>
       </c>
       <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:49:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1274,8 +1274,49 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Kan mijn wachtwoord niet resetten</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Ik krijg geen e-mail bij wachtwoord resetten.</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Het spijt me te horen dat u geen e-mail heeft ontvangen bij het resetten van uw wachtwoord. Om dit probleem zo snel mogelijk voor u op te lossen, zou u ons alstublieft uw gebruikersnaam willen doorgeven? Op die manier kunnen we gerichter onderzoeken waar het probleem zich voordoet en u verder helpen.
+Ik kijk ernaar uit om uw gegevens te ontvangen, zodat we dit snel kunnen oplossen.
+Met vriendelijke groet,
+[Naam] E-mailassistent at [Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:49:12</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1295,7 +1336,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1340,7 +1381,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:50:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1315,8 +1315,49 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Aanmelden voor beurs</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Wij willen graag deelnemen aan de komende vakbeurs.</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Beste,
+Bedankt voor uw interesse in deelname aan de komende vakbeurs. Voor meer informatie over de mogelijkheden en beschikbaarheid verzoek ik u vriendelijk om contact op te nemen met onze evenementencoördinator via [contactgegevens]. Hij/zij zal u verder kunnen informeren over de beschikbare standruimte, kosten en eventuele inschrijvingsprocedure.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:50:16</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D19">
+  <conditionalFormatting sqref="D2:D20">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1336,7 +1377,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1417,17 +1458,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Uitnodiging / Evenement</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1437,7 +1478,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Uitnodiging / Evenement</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1447,7 +1488,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1457,7 +1498,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B10" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:51:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$12</f>
+              <f>'Dashboard'!$A$2:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$12</f>
+              <f>'Dashboard'!$B$2:$B$13</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1356,8 +1356,52 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Verzoek om factuur</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Kunt u mij een factuur sturen voor mijn laatste bestelling?</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Om u te kunnen helpen met het versturen van een factuur voor uw laatste bestelling, hebben wij wat extra informatie nodig. Kunt u ons alstublieft de volgende gegevens verstrekken:
+1. Uw bestelnummer
+2. De datum van uw bestelling
+3. Het e-mailadres waarnaar wij de factuur kunnen sturen
+Zodra wij deze gegevens van u hebben ontvangen, zullen wij zo spoedig mogelijk de factuur voor u opstellen en toesturen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:51:15</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1377,7 +1421,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1395,7 +1439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1438,7 +1482,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1448,7 +1492,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1458,7 +1502,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1488,7 +1532,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1498,7 +1542,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1508,7 +1552,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1518,10 +1562,20 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:52:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$13</f>
+              <f>'Dashboard'!$A$2:$A$14</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$13</f>
+              <f>'Dashboard'!$B$2:$B$14</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1400,8 +1400,40 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Status van mijn bestelling</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Wanneer wordt mijn bestelling bezorgd?</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:52:13</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1421,7 +1453,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1439,7 +1471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1482,7 +1514,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1492,7 +1524,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1512,7 +1544,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1532,7 +1564,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1542,7 +1574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1552,7 +1584,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1562,7 +1594,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1576,6 +1608,16 @@
         </is>
       </c>
       <c r="B13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:53:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1432,8 +1432,40 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Aanmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Ik wil me graag inschrijven voor de nieuwsbrief.</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:53:13</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D22">
+  <conditionalFormatting sqref="D2:D23">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1453,7 +1485,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22">
+  <conditionalFormatting sqref="G2:G23">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1544,17 +1576,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Uitnodiging / Evenement</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1574,7 +1606,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Uitnodiging / Evenement</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1594,7 +1626,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B12" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:54:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1464,8 +1464,49 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Offerte voor 500 stuks</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Graag ontvang ik een offerte voor 500 stuks van product X.</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u wel voor uw interesse in product X. Om u een offerte op maat te kunnen sturen, hebben wij wat meer informatie nodig. Kunt u ons laten weten welke specifieke variant(en) van product X u wenst te bestellen en in welke regio de levering zal plaatsvinden? Op basis van deze gegevens kunnen wij een passende offerte voor u opstellen.
+Alvast bedankt voor de aanvullende informatie.
+Met vriendelijke groet,
+[Naam Bedrijf]</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:54:34</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D23">
+  <conditionalFormatting sqref="D2:D24">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1485,7 +1526,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G23">
+  <conditionalFormatting sqref="G2:G24">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1556,7 +1597,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1566,7 +1607,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1576,7 +1617,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1586,11 +1627,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -1616,7 +1657,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1626,7 +1667,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B12" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:55:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1505,8 +1505,40 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Aanmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Ik wil me graag inschrijven voor de nieuwsbrief.</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:55:11</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D24">
+  <conditionalFormatting sqref="D2:D25">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1526,7 +1558,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G24">
+  <conditionalFormatting sqref="G2:G25">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1587,17 +1619,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1607,7 +1639,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1627,7 +1659,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:56:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1537,8 +1537,40 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Ruilen van product</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Kan ik dit product ruilen voor een andere maat?</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:56:13</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D25">
+  <conditionalFormatting sqref="D2:D26">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1558,7 +1590,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G25">
+  <conditionalFormatting sqref="G2:G26">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1649,7 +1681,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1659,7 +1691,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1669,17 +1701,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Uitnodiging / Evenement</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1699,7 +1731,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Uitnodiging / Evenement</t>
         </is>
       </c>
       <c r="B12" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:57:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$14</f>
+              <f>'Dashboard'!$A$2:$A$15</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$14</f>
+              <f>'Dashboard'!$B$2:$B$15</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1569,8 +1569,51 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Privacybeleid</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Wat doen jullie met klantgegevens volgens GDPR?</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Juridisch / Contract</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw vraag over hoe wij omgaan met klantgegevens volgens de GDPR. Wij nemen de privacy en bescherming van persoonlijke gegevens van onze klanten uiterst serieus en volgen hierbij strikt de richtlijnen van de Algemene Verordening Gegevensbescherming (AVG/GDPR).
+Om uw privacy te waarborgen, zorgen wij ervoor dat alle klantgegevens veilig worden opgeslagen en verwerkt volgens de geldende wet- en regelgeving. Dit houdt in dat we alleen persoonlijke gegevens verzamelen die relevant zijn voor het leveren van onze diensten en dat we deze gegevens niet delen met derden zonder uw toestemming, tenzij dit noodzakelijk is voor de uitvoering van onze diensten.
+Mocht u nog specifieke vragen hebben over hoe wij omgaan met uw gegevens of wilt u meer informatie ontvangen, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam] Nederlandse e-mailassistent 
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:57:33</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="D2:D27">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1590,7 +1633,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
+  <conditionalFormatting sqref="G2:G27">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1608,7 +1651,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1641,7 +1684,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1651,7 +1694,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1661,7 +1704,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1671,7 +1714,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1681,7 +1724,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1701,7 +1744,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1721,7 +1764,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Uitnodiging / Evenement</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1731,7 +1774,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Uitnodiging / Evenement</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1755,6 +1798,16 @@
         </is>
       </c>
       <c r="B14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Juridisch / Contract</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:58:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1612,8 +1612,51 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Onjuiste bestelling</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Ik heb een ander product ontvangen dan ik had besteld.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw bericht. We vinden het vervelend om te horen dat u een ander product heeft ontvangen dan u had besteld. Om dit probleem op te lossen, willen we u vragen om het volgende te doen:
+1. Stuur ons alstublieft een foto van het ontvangen product, samen met uw bestelnummer, naar ons e-mailadres, zodat we dit kunnen verifiëren.
+2. Geef ons ook de omschrijving van het product dat u had besteld, zodat we het verschil kunnen vaststellen.
+Zodra we deze informatie hebben ontvangen, zullen we ons best doen om dit zo snel mogelijk voor u op te lossen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:58:15</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D27">
+  <conditionalFormatting sqref="D2:D28">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1633,7 +1676,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G27">
+  <conditionalFormatting sqref="G2:G28">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1694,7 +1737,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1704,11 +1747,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -1744,7 +1787,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B9" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 18:59:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1655,8 +1655,48 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Vragen over handleiding</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Waar kan ik de handleiding van product X vinden?</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw vraag. De handleiding van product X is te vinden op onze website onder de rubriek 'Ondersteuning' of 'Downloads'. Mocht u hier hulp bij nodig hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam] - Klantenservice</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-06-22 18:59:16</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D28">
+  <conditionalFormatting sqref="D2:D29">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1676,7 +1716,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G28">
+  <conditionalFormatting sqref="G2:G29">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1727,17 +1767,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1747,7 +1787,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 19:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1695,8 +1695,40 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-06-22 19:00:14</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
+  <conditionalFormatting sqref="D2:D30">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1716,7 +1748,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G29">
+  <conditionalFormatting sqref="G2:G30">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1777,7 +1809,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1787,7 +1819,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1797,11 +1829,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -1827,7 +1859,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B9" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 19:01:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1727,8 +1727,49 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Retour is nog niet verwerkt</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Ik heb iets teruggestuurd maar hoor niks. Wanneer krijg ik mijn geld terug?</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Om je vraag over de terugbetaling te kunnen beantwoorden, hebben we wat meer informatie nodig. Zou je ons alsjeblieft je ordernummer kunnen sturen, zodat we dit kunnen nakijken in ons systeem? Op die manier kunnen we controleren of de retourzending is ontvangen en de terugbetaling is verwerkt.
+We doen ons best om je zo snel mogelijk van dienst te zijn. Bedankt voor je geduld en medewerking.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-06-22 19:01:16</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D30">
+  <conditionalFormatting sqref="D2:D31">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1748,7 +1789,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G30">
+  <conditionalFormatting sqref="G2:G31">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1813,7 +1854,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 19:02:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1768,8 +1768,52 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>B2B samenwerkingsvoorstel</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Ik wil graag een samenwerking bespreken voor onze zakelijke klanten.</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Geachte heer/mevrouw,
+Hartelijk dank voor uw interesse in een mogelijke samenwerking met ons bedrijf voor onze zakelijke klanten. Wij waarderen uw voorstel en willen graag meer informatie ontvangen om te bekijken hoe we kunnen samenwerken.
+Kunt u meer details verstrekken over uw bedrijf en de diensten die u aanbiedt? Op basis hiervan kunnen we beoordelen of er mogelijkheden zijn voor een vruchtbare samenwerking.
+Ik kijk uit naar uw antwoord.
+Met vriendelijke groet,
+[Naam]  
+E-mailassistent  
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2025-06-22 19:02:34</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D31">
+  <conditionalFormatting sqref="D2:D32">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1789,7 +1833,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G31">
+  <conditionalFormatting sqref="G2:G32">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1840,7 +1884,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1860,17 +1904,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 19:03:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1812,8 +1812,49 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Offerte voor 500 stuks</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Graag ontvang ik een offerte voor 500 stuks van product X.</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Hartelijk dank voor uw interesse in product X. Om u een nauwkeurige offerte te kunnen sturen, hebben we wat meer informatie nodig. Kunt u ons laten weten of u specifieke eisen heeft met betrekking tot het product of de levering? Ook is het handig als u de gewenste leverdatum kunt vermelden.
+Zodra we deze details van u ontvangen, zullen we zo spoedig mogelijk een offerte voor 500 stuks van product X opstellen.
+Met vriendelijke groet,
+[Naam van het bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2025-06-22 19:03:12</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D32">
+  <conditionalFormatting sqref="D2:D33">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1833,7 +1874,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G32">
+  <conditionalFormatting sqref="G2:G33">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1924,11 +1965,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -1944,7 +1985,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B9" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 19:04:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1853,8 +1853,50 @@
         </is>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Technische storing</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>De website werkt niet goed. Is hier iets mis mee?</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Om het probleem beter te kunnen onderzoeken, hebben we meer informatie nodig. Zou je alsjeblieft kunnen aangeven welke specifieke problemen je ervaart wanneer je de website probeert te gebruiken? Bijvoorbeeld, krijg je een foutmelding te zien of lukt het niet om in te loggen? Met deze details kunnen we het probleem gericht aanpakken en een oplossing bieden.
+We horen graag meer van je, zodat we je verder kunnen helpen.
+Met vriendelijke groet,  
+[Tekstschrijver]  
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2025-06-22 19:04:33</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D33">
+  <conditionalFormatting sqref="D2:D34">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1874,7 +1916,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G33">
+  <conditionalFormatting sqref="G2:G34">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1919,7 +1961,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 19:05:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1895,8 +1895,48 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie geopend?</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw vraag. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. Op zaterdag zijn wij gesloten. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2025-06-22 19:05:12</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D34">
+  <conditionalFormatting sqref="D2:D35">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1916,7 +1956,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G34">
+  <conditionalFormatting sqref="G2:G35">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2027,7 +2067,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2037,17 +2077,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Uitnodiging / Evenement</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -2057,7 +2097,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Uitnodiging / Evenement</t>
         </is>
       </c>
       <c r="B12" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 19:06:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1935,8 +1935,49 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Privacybeleid</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Wat doen jullie met klantgegevens volgens GDPR?</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Juridisch / Contract</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank u wel voor uw vraag over ons beleid met betrekking tot klantgegevens volgens de GDPR. Bij ons bedrijf nemen wij de bescherming van persoonlijke gegevens zeer serieus. Wij voldoen aan de eisen en verplichtingen van de Algemene verordening gegevensbescherming (AVG) om ervoor te zorgen dat alle klantgegevens veilig en vertrouwelijk worden behandeld.
+Als u meer specifieke informatie wenst over hoe wij omgaan met klantgegevens of als u wilt weten welke gegevens wij precies verzamelen en hoe we die gebruiken, dan kunt u contact met ons opnemen. 
+Met vriendelijke groet,
+[Bedrijfsnaam] Beveiliging &amp; Compliance Team</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2025-06-22 19:06:35</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D35">
+  <conditionalFormatting sqref="D2:D36">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1956,7 +1997,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G35">
+  <conditionalFormatting sqref="G2:G36">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2067,7 +2108,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Juridisch / Contract</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2087,11 +2128,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -2107,7 +2148,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -2117,7 +2158,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -2127,7 +2168,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Juridisch / Contract</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B15" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 19:07:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1976,8 +1976,48 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Sollicitatie salesfunctie</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Hierbij mijn sollicitatie voor de salesfunctie. CV in bijlage.</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Beste sollicitant,
+Dank voor het sturen van je sollicitatie voor de salesfunctie. We zullen je CV zorgvuldig bekijken en zo spoedig mogelijk contact met je opnemen over de vervolgstappen. Mocht je in de tussentijd vragen hebben, dan horen we het graag.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2025-06-22 19:07:11</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D36">
+  <conditionalFormatting sqref="D2:D37">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1997,7 +2037,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G36">
+  <conditionalFormatting sqref="G2:G37">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2078,7 +2118,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2088,7 +2128,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2098,17 +2138,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Juridisch / Contract</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2118,7 +2158,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -2128,7 +2168,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Juridisch / Contract</t>
         </is>
       </c>
       <c r="B11" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 19:09:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2016,8 +2016,88 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Sollicitatie salesfunctie</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Hierbij mijn sollicitatie voor de salesfunctie. CV in bijlage.</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Beste,
+Bedankt voor je sollicitatie voor de salesfunctie. We waarderen je interesse in ons bedrijf. Ik zal je CV zorgvuldig bekijken en contact met je opnemen als er verdere stappen nodig zijn.
+Met vriendelijke groet,
+[Naam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2025-06-22 19:09:11</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Vragen over nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Wanneer wordt de volgende nieuwsbrief verstuurd?</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank voor je interesse in onze nieuwsbrief. De volgende nieuwsbrief staat gepland om aanstaande vrijdag te worden verstuurd. Houd dus je inbox in de gaten!
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2025-06-22 19:09:14</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D37">
+  <conditionalFormatting sqref="D2:D39">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2037,7 +2117,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G37">
+  <conditionalFormatting sqref="G2:G39">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2088,7 +2168,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2098,7 +2178,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2108,7 +2188,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2118,27 +2198,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 19:10:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2096,8 +2096,49 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Technische storing</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>De website werkt niet goed. Is hier iets mis mee?</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor het melden van dit probleem. Om dit verder te onderzoeken, heb ik wat meer informatie van u nodig. Kunt u specifiek aangeven welke problemen u ondervindt wanneer u de website bezoekt? Ziet u foutmeldingen, laadt de pagina niet, of zijn bepaalde functies niet beschikbaar? Alle details die u kunt geven zullen ons helpen het probleem op te lossen. 
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2025-06-22 19:10:15</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D39">
+  <conditionalFormatting sqref="D2:D40">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2117,7 +2158,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G39">
+  <conditionalFormatting sqref="G2:G40">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2162,7 +2203,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 19:11:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2137,8 +2137,48 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Kan mijn wachtwoord niet resetten</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Ik krijg geen e-mail bij wachtwoord resetten.</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw e-mail. Om het probleem met het niet ontvangen van e-mails voor het resetten van uw wachtwoord op te lossen, hebben we wat meer informatie nodig. Zou u ons alstublieft de gebruikersnaam of het e-mailadres kunnen geven waarvoor u het wachtwoord wilt resetten? Op deze manier kunnen we verder onderzoeken waar het probleem precies ligt en u van dienst zijn.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2025-06-22 19:11:15</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D40">
+  <conditionalFormatting sqref="D2:D41">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2158,7 +2198,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G40">
+  <conditionalFormatting sqref="G2:G41">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2203,7 +2243,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 21:37:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2177,8 +2177,40 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Open sollicitatie</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Zijn er op dit moment openstaande functies bij jullie bedrijf?</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>2025-06-22 21:37:13</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D41">
+  <conditionalFormatting sqref="D2:D42">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2198,7 +2230,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G41">
+  <conditionalFormatting sqref="G2:G42">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2253,7 +2285,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 21:39:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2209,8 +2209,48 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Verzoek om factuur</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Kunt u mij een factuur sturen voor mijn laatste bestelling?</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je e-mail. Om je te helpen met de factuur voor je laatste bestelling, heb ik wat meer informatie nodig. Zou je mij alsjeblieft de volgende gegevens kunnen doorgeven: ordernummer en/of datum van de bestelling? Zodra ik deze gegevens heb ontvangen, zal ik ervoor zorgen dat de factuur naar je wordt verstuurd.
+Met vriendelijke groet,
+[Naam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2025-06-22 21:39:22</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D42">
+  <conditionalFormatting sqref="D2:D43">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2230,7 +2270,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G42">
+  <conditionalFormatting sqref="G2:G43">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2361,7 +2401,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Juridisch / Contract</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -2371,11 +2411,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Uitnodiging / Evenement</t>
+          <t>Juridisch / Contract</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -2391,7 +2431,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Uitnodiging / Evenement</t>
         </is>
       </c>
       <c r="B14" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 21:41:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2249,8 +2249,48 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Korting voor wederverkopers?</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Biedt u speciale prijzen voor wederverkopers?</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw interesse in onze producten. Ja, wij bieden speciale prijzen aan voor wederverkopers. Om hier meer informatie over te krijgen en om te weten te komen hoe wij u verder kunnen helpen, kunt u het beste contact opnemen met ons verkoopteam via verkoop@bedrijfsnaam.nl.
+Met vriendelijke groet,
+[Bedrijfsnaam] Team</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2025-06-22 21:41:26</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D43">
+  <conditionalFormatting sqref="D2:D44">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2270,7 +2310,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G43">
+  <conditionalFormatting sqref="G2:G44">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2331,7 +2371,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2371,11 +2411,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 21:43:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2289,8 +2289,53 @@
         </is>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Mijn bestelling is incompleet geleverd. Graag hoor ik hoe dit wordt opgelost.</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Mijn excuses dat uw bestelling incompleet is geleverd. Om dit voor u op te lossen, heb ik wat meer informatie nodig. Kunt u mij alstublieft het volgende verstrekken:
+- Uw bestelnummer
+- De ontbrekende item(s)
+Met deze gegevens kan ik direct voor u nakijken wat er mis is gegaan en een passende oplossing bieden.
+Ik hoor graag van u.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2025-06-22 21:43:42</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D44">
+  <conditionalFormatting sqref="D2:D45">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2310,7 +2355,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G44">
+  <conditionalFormatting sqref="G2:G45">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2451,7 +2496,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Juridisch / Contract</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -2461,11 +2506,11 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Juridisch / Contract</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -2481,7 +2526,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B15" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 21:46:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2334,8 +2334,48 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Sollicitatie salesfunctie</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Hierbij mijn sollicitatie voor de salesfunctie. CV in bijlage.</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Beste sollicitant,
+Dank u voor uw interesse in de salesfunctie bij ons bedrijf. We hebben uw sollicitatie en CV ontvangen. Onze HR-afdeling zal uw sollicitatie zo spoedig mogelijk bekijken en contact met u opnemen indien uw profiel aansluit bij de functievereisten.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2025-06-22 21:45:50</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D45">
+  <conditionalFormatting sqref="D2:D46">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2355,7 +2395,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G45">
+  <conditionalFormatting sqref="G2:G46">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2410,7 +2450,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 21:51:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2374,8 +2374,81 @@
         </is>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Technische storing</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>De website werkt niet goed. Is hier iets mis mee?</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw bericht. Om het probleem met de website te kunnen onderzoeken, hebben we wat meer informatie nodig. Kunt u specifiek aangeven welke functionaliteit of pagina niet goed werkt? Zijn er foutmeldingen die u ziet? Eventuele details die u kunt verstrekken, zoals de browser die u gebruikt, kunnen ook van pas komen. Met deze gegevens kunnen we het probleem beter identificeren en u hopelijk sneller helpen.
+Alvast bedankt voor uw medewerking.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2025-06-22 21:51:13</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Retour is nog niet verwerkt</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Ik heb iets teruggestuurd maar hoor niks. Wanneer krijg ik mijn geld terug?</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>2025-06-22 21:51:14</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D46">
+  <conditionalFormatting sqref="D2:D48">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2395,7 +2468,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G46">
+  <conditionalFormatting sqref="G2:G48">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2440,7 +2513,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -2456,17 +2529,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2476,7 +2549,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2486,7 +2559,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B7" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 21:53:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2447,8 +2447,48 @@
         </is>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Offerte voor 500 stuks</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Graag ontvang ik een offerte voor 500 stuks van product X.</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw interesse in product X. Om een offerte voor 500 stuks te kunnen opstellen, hebben we meer informatie nodig. Kunt u de specificaties van het product en eventuele voorkeuren doorgeven, zoals kleur, maat, en eventuele extra functies? Nadat we deze gegevens hebben ontvangen, zullen we zo spoedig mogelijk een offerte voor u opstellen.
+Met vriendelijke groet,
+[Naam] - E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2025-06-22 21:53:21</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D48">
+  <conditionalFormatting sqref="D2:D49">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2468,7 +2508,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G48">
+  <conditionalFormatting sqref="G2:G49">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2529,7 +2569,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2539,11 +2579,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 21:55:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2487,8 +2487,40 @@
         </is>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Beschadigd product ontvangen</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Het product dat ik heb ontvangen is beschadigd aangekomen.</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2025-06-22 21:55:42</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D49">
+  <conditionalFormatting sqref="D2:D50">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2508,7 +2540,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G49">
+  <conditionalFormatting sqref="G2:G50">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2569,17 +2601,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 21:58:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2519,8 +2519,49 @@
         </is>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Kan mijn wachtwoord niet resetten</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Ik krijg geen e-mail bij wachtwoord resetten.</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor het melden van dit probleem. Om u verder te kunnen helpen, hebben we enkele aanvullende gegevens nodig. Kunt u ons uw gebruikersnaam of het e-mailadres waarmee u probeerde uw wachtwoord opnieuw in te stellen, geven? Op die manier kunnen we het probleem gericht onderzoeken en oplossen.
+Alvast bedankt voor uw medewerking.
+Met vriendelijke groet,
+[Naam bedrijf] - E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>2025-06-22 21:58:13</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D50">
+  <conditionalFormatting sqref="D2:D51">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2540,7 +2581,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G50">
+  <conditionalFormatting sqref="G2:G51">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2585,7 +2626,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 22:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2560,8 +2560,48 @@
         </is>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Is product Y nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Ik wil graag weten of product Y beschikbaar is.</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank je wel voor je interesse in product Y. Helaas is product Y momenteel niet op voorraad. We verwachten een nieuwe levering binnen twee weken. Mocht je op de hoogte gehouden willen worden wanneer het product weer beschikbaar is, laat het ons dan weten.
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2025-06-22 22:00:21</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D51">
+  <conditionalFormatting sqref="D2:D52">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2581,7 +2621,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G51">
+  <conditionalFormatting sqref="G2:G52">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2662,11 +2702,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -2682,7 +2722,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 22:02:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2600,8 +2600,49 @@
         </is>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Onjuiste bestelling</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Ik heb een ander product ontvangen dan ik had besteld.</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw bericht. Mijn excuses voor het ongemak dat u heeft ervaren. Om dit probleem snel op te lossen, zou u alstublieft wat meer details kunnen geven over het verkeerd ontvangen product en het product dat u eigenlijk had besteld? Zo kunnen we dit verder onderzoeken en een passende oplossing vinden.
+We kijken uit naar uw reactie.
+Met vriendelijke groet,
+[Naam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>2025-06-22 22:02:45</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D52">
+  <conditionalFormatting sqref="D2:D53">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2621,7 +2662,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G52">
+  <conditionalFormatting sqref="G2:G53">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2672,17 +2713,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 22:05:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2641,8 +2641,40 @@
         </is>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Order wijzigen</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Kan ik mijn bestelling nog aanpassen?</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>2025-06-22 22:05:11</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D53">
+  <conditionalFormatting sqref="D2:D54">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2662,7 +2694,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G53">
+  <conditionalFormatting sqref="G2:G54">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2773,11 +2805,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -2793,7 +2825,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -2803,7 +2835,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B12" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 22:07:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2673,8 +2673,49 @@
         </is>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>BTW-nummer toevoegen</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Mijn BTW-nummer is niet vermeld op de factuur.</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank u voor uw bericht. Om uw probleem met betrekking tot het ontbrekende BTW-nummer op de factuur op te lossen, ontvangen wij graag meer informatie om uw specifieke situatie te begrijpen. Kunt u ons uw factuurnummer en bedrijfsnaam doorgeven, zodat wij dit verder kunnen onderzoeken en indien nodig corrigeren?
+Wij streven ernaar om u zo snel mogelijk van dienst te zijn en verontschuldigen ons voor het ongemak.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>2025-06-22 22:07:17</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D54">
+  <conditionalFormatting sqref="D2:D55">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2694,7 +2735,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G54">
+  <conditionalFormatting sqref="G2:G55">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2805,7 +2846,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2815,17 +2856,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -2835,7 +2876,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B12" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 22:09:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2714,8 +2714,48 @@
         </is>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Inlogproblemen</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Ik kan niet meer inloggen op mijn account. Kunnen jullie helpen?</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Om je verder te kunnen helpen met het inlogprobleem, hebben we wat meer informatie nodig. Zou je alsjeblieft je gebruikersnaam en eventuele foutmeldingen die je hebt ontvangen kunnen delen? Op die manier kunnen we het probleem zo snel mogelijk voor je oplossen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>2025-06-22 22:09:26</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D55">
+  <conditionalFormatting sqref="D2:D56">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2735,7 +2775,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G55">
+  <conditionalFormatting sqref="G2:G56">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2780,7 +2820,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 22:11:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2754,8 +2754,49 @@
         </is>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Status van mijn bestelling</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Wanneer wordt mijn bestelling bezorgd?</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je e-mail. Om de status van je bestelling te controleren en meer te weten te komen over de verwachte bezorgdatum, heb ik je bestelnummer nodig. Zou je zo vriendelijk willen zijn om je bestelnummer met mij te delen, zodat ik dit verder voor je kan nakijken?
+Ik hoor graag van je om je verder te helpen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>2025-06-22 22:11:31</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D56">
+  <conditionalFormatting sqref="D2:D57">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2775,7 +2816,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G56">
+  <conditionalFormatting sqref="G2:G57">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2876,7 +2917,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -2886,17 +2927,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B10" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 22:13:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2795,8 +2795,40 @@
         </is>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Ruilen van product</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Kan ik dit product ruilen voor een andere maat?</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>2025-06-22 22:13:34</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D57">
+  <conditionalFormatting sqref="D2:D58">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2816,7 +2848,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G57">
+  <conditionalFormatting sqref="G2:G58">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2871,7 +2903,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 22:15:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2827,8 +2827,48 @@
         </is>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Herinnering betaling</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Ik zie dat ik nog een openstaande betaling heb. Kunt u dit bevestigen?</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Om u verder te kunnen helpen, heb ik wat meer informatie nodig om uw openstaande betaling te verifiëren. Kunt u mij alstublieft uw factuurnummer en/of klantnummer doorgeven? Zodra ik deze gegevens heb, zal ik direct voor u nakijken of er inderdaad nog een openstaande betaling is.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>2025-06-22 22:15:44</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D58">
+  <conditionalFormatting sqref="D2:D59">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2848,7 +2888,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G58">
+  <conditionalFormatting sqref="G2:G59">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2949,7 +2989,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -2959,7 +2999,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2969,11 +3009,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 22:17:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2867,8 +2867,49 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Retour aanmelden</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Ik wil graag een artikel retourneren. Hoe werkt dat?</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Om een artikel te retourneren, verzoeken we je om contact met ons op te nemen via onze klantenservice of het retourformulier op onze website in te vullen. Vermeld hierbij het ordernummer en de reden van retour. 
+Zodra we deze informatie hebben ontvangen, nemen we contact met je op om de retourzending verder af te handelen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>2025-06-22 22:17:48</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D59">
+  <conditionalFormatting sqref="D2:D60">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2888,7 +2929,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G59">
+  <conditionalFormatting sqref="G2:G60">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2943,7 +2984,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-22 22:20:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-22.xlsx
+++ b/logs/mail_log_2025-06-22.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2908,8 +2908,49 @@
         </is>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Wat is het verschil tussen product A en product B?</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw interesse in onze producten A en B. Product A heeft een grotere capaciteit en meer geavanceerde functies dan product B. Product B daarentegen is compacter en eenvoudiger in gebruik. Afhankelijk van uw behoeften en budget kunt u kiezen welk product het beste bij u past.
+Mocht u nog specifieke vragen hebben over de functies van beide producten, dan helpen wij u graag verder.
+Met vriendelijke groet,
+[Naam van het bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>2025-06-22 22:19:53</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D60">
+  <conditionalFormatting sqref="D2:D61">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2929,7 +2970,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G60">
+  <conditionalFormatting sqref="G2:G61">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2990,7 +3031,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -3000,17 +3041,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>